<commit_message>
Update Eric's timesheet for week 7
</commit_message>
<xml_diff>
--- a/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Ka Yiu Eric Ma.xlsx
+++ b/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Ka Yiu Eric Ma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Google Drive/U Adelaide course materials/MCI projects/Team-024/Time sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Google Drive/U Adelaide course materials/MCI projects/Team-024/Agenda_Minutes_Timesheet/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D875B-A01D-7D40-8341-F0A1D515CF72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960247C5-B9EF-2542-92C6-FE817393EFEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Week 6" sheetId="8" r:id="rId6"/>
     <sheet name="Sem Break Week 1" sheetId="9" r:id="rId7"/>
     <sheet name="Sem Break Week 2" sheetId="10" r:id="rId8"/>
+    <sheet name="Week 7" sheetId="12" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Sem Break Week 1'!$A$1:$H$13</definedName>
@@ -31,6 +32,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Week 4'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Week 5'!$A$1:$H$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Week 6'!$A$1:$H$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Week 7'!$A$1:$H$13</definedName>
     <definedName name="Week_Start" localSheetId="6">'Sem Break Week 1'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="7">'Sem Break Week 2'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="0">'Week 1'!$C$4</definedName>
@@ -38,6 +40,7 @@
     <definedName name="Week_Start" localSheetId="3">'Week 4'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="4">'Week 5'!$C$4</definedName>
     <definedName name="Week_Start" localSheetId="5">'Week 6'!$C$4</definedName>
+    <definedName name="Week_Start" localSheetId="8">'Week 7'!$C$4</definedName>
     <definedName name="Week_Start">'Week 3'!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="80">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -281,6 +284,24 @@
   </si>
   <si>
     <t>Fix bug in home page that the http request of loading sample data triggers only once</t>
+  </si>
+  <si>
+    <t>Fix bug found in client meeting - not be to update data loaded from backend to present in Home page</t>
+  </si>
+  <si>
+    <t>Fix the bug and Jason will work on a video recording sending to client showing that the bug has been fixed</t>
+  </si>
+  <si>
+    <t>Complete 80% of the online course for ionic Framework with Angular at Udemy</t>
+  </si>
+  <si>
+    <t>Work on adding new acitivies implemented and reflection about managing problems in milestone 1 report</t>
+  </si>
+  <si>
+    <t>As part of the milestone 1 report</t>
+  </si>
+  <si>
+    <t>Complete adding new acitivies implemented and reflection about managing problems in milestone 1 report</t>
   </si>
 </sst>
 </file>
@@ -502,11 +523,11 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -870,16 +891,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1333,16 +1354,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1808,7 +1829,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1824,16 +1845,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2291,7 +2312,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2307,16 +2328,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2798,16 +2819,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3273,7 +3294,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A2" sqref="A2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3289,16 +3310,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3764,7 +3785,7 @@
   <dimension ref="A2:AW12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3780,16 +3801,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3807,7 +3828,7 @@
       <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4268,8 +4289,8 @@
   </sheetPr>
   <dimension ref="A2:AW12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4285,16 +4306,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4312,7 +4333,7 @@
       <c r="G3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>54</v>
       </c>
     </row>
@@ -4764,4 +4785,495 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80153E0B-FAF9-204E-85FB-B14883817239}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:AW12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="15" max="49" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:49" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1792052</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:49" s="14" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+    </row>
+    <row r="7" spans="1:49" s="14" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="20">
+        <v>44313</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E7" s="12">
+        <v>4</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+    </row>
+    <row r="8" spans="1:49" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="20">
+        <v>44314</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="12">
+        <v>8</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13"/>
+      <c r="AM8" s="13"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
+      <c r="AP8" s="13"/>
+      <c r="AQ8" s="13"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+    </row>
+    <row r="9" spans="1:49" s="14" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="20">
+        <v>44315</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E9" s="12">
+        <v>6</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AQ9" s="13"/>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+    </row>
+    <row r="10" spans="1:49" s="14" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="20">
+        <v>44316</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="13"/>
+      <c r="AQ10" s="13"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+    </row>
+    <row r="11" spans="1:49" s="14" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+    </row>
+    <row r="12" spans="1:49" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8">
+        <f>SUM(E6:E11)</f>
+        <v>21</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C6:D11" xr:uid="{FA991B5F-7F4C-754A-A57A-5E443DAFF686}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="98" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>